<commit_message>
Adding my weekly work
</commit_message>
<xml_diff>
--- a/weeklyWorkBreakdown.xlsx
+++ b/weeklyWorkBreakdown.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46c66270056a4b13/Documents/UWE_CS_Y2/SD/GroupProject/systems-development-group-work/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\William Forber\Documents\Computer science\Year 2\Systems Development\systems-development-group-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{B80EE0D6-C86F-4575-BA09-719007FB3772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83A32520-C827-4AC9-8F22-7E58F33EF255}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A591A439-09BC-4528-B17C-345BD0CB37EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{03EAD80C-C4E7-4730-A8C5-4CE6BE603DD2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{03EAD80C-C4E7-4730-A8C5-4CE6BE603DD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Lewis</t>
   </si>
@@ -99,13 +99,34 @@
   </si>
   <si>
     <t>Write Evaluation</t>
+  </si>
+  <si>
+    <t>Lit Review</t>
+  </si>
+  <si>
+    <t>Aims and objectives + Class and sequance diagrams</t>
+  </si>
+  <si>
+    <t>Sidebar GUI</t>
+  </si>
+  <si>
+    <t>Filtering</t>
+  </si>
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>Machine learning</t>
+  </si>
+  <si>
+    <t>Implementation report</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,12 +240,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,89 +583,109 @@
   <dimension ref="B2:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="12" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20.75" customWidth="1"/>
+    <col min="4" max="4" width="52.75" customWidth="1"/>
+    <col min="5" max="5" width="20.75" customWidth="1"/>
+    <col min="6" max="6" width="24.25" customWidth="1"/>
+    <col min="7" max="12" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="2:12">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4" t="s">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5" t="s">
+      <c r="I3" s="7"/>
+      <c r="J3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -659,7 +700,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -674,7 +715,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
@@ -697,5 +738,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>